<commit_message>
HOTFIX: added wakeup and fixed local path to file
</commit_message>
<xml_diff>
--- a/backend/records.xlsx
+++ b/backend/records.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:Q20"/>
@@ -623,6 +623,109 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4635434752</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Zora</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/07/IMG_6238-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Via een inbeslagname is Zora in ons asiel binnengekomen en uiteindelijk ook toegewezen.
+Ze heeft tijd nodig gehad om de mensen van het asiel te leren kennen, vanaf het moment dat het ijs was gebroken, is Zora een erg aanhankelijke hond voor de mensen die ze kent.
+Werken wil Zora wel en spelen is ook zeker een hobby. Je hebt haar volledige aandacht wanneer je lekkere vleesjes hebt en dan merk je ook dat ze de basiscommando’s van thuis uit kent. Ze kent de commando’s ‘zit, ‘liggen’, ‘poot’ en ‘blijf’ en gezien haar leergierigheid, weten we zeker dat ze véél meer commando’s kan leren.
+Zora wil ook graag samen spelen en als ze wil dat je iets gooit komt ze het speeltje op je schoot leggen.
+Zora wordt wel het best met rust gelaten tijdens het eten of wanneer ze lekker rustig ligt te knabbelen op een kauwbotje. Ze heeft moeite met vreemde mensen en andere dieren dus hier moet de nieuwe eigenaar zeker rekening mee houden. We zoeken een thuis met mensen die het Mechelse herder ras kennen. Daarnaast een huis met een goed afgesloten tuin zonder kinderen of andere dieren.
+</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Vicky</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/04/vickyyy-1-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Er zijn zo van die honden die bijna horen tot het ‘vaste meubilair’ van het asiel. Zonde, want we begrijpen vaak zelf niet goed hoe dat komt.
+Een van die honden is Mechelaar Vicky.
+Deze 7-jarige dame zit al bijna 3 jaar in ons asiel en ze zit samen met Molly in onze top drie van langzitters. Haar blinkende ogen verraden weinig over haar trieste verleden. Vicky’s leefruimte beperkte zich namelijk lang tot enkel een vieze ren.
+Vicky is ontzettend aanhankelijk, slim, energiek en speels. Ze houdt enorm van aandacht, maar heeft nog niet helemaal door dat je die best netjes vraagt. Aan de etiquette moet dus nog wat gewerkt worden. Je ziet Vicky heerlijk genieten van aaien, maar het allergelukkigste maak je haar door samen actief te zijn.
+Samen spelen in de tuin, speuren of trainen vindt ze heerlijk.
+Vicky is al goed getraind en doet het steeds beter aan de riem. Je begint wel best met wandelen in een rustige, prikkelarme omgeving. Het leven in huis kent ze nog niet, dus ze weet ook nog niet hoe ze met spullen in huis moet omgaan. Maar met het nodige geduld, leert slimme Vicky vast wel hoe ze zich als een echte dame moet gedragen.
+Vicky kan niet bij andere dieren of kleine kinderen. Ze heeft ook nood aan een grote omheinde tuin om lekker in rond te rennen. 
+Zoek je een energiek, aanhankelijk maatje dat je eerst vanop een veilig plekje kunt laten wennen aan het leven in huis? Dan is Vicky misschien wel de geknipte hond voor jou!
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Storm</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/07/IMG_7123-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Storm werd in beslag genomen omdat ze aan een boom werd vastgebonden. Storm heeft voordat ze in beslag werd genomen 2 andere eigenaren gehad.
+Storm haar oren werken prima, wanneer zij daar zin in heeft. Wanneer ze aan het snuffelen is en ze geroepen wordt, zal ze haar gehoor even uitzetten. Zijn er lekkere snoepjes te verdienen? Kom maar op!
+Deze prachtige dame is gek op eten en is daardoor ook leergierig. Er zit ook een keerzijde van haar passie voor eten: ze durft eten en objecten die zij als belangrijk ziet te beschermen.
+Storm vindt het niet fijn wanneer we haar aanlijnen. We vermoeden dat haar verleden, waarbij ze aangelijnd aan een boom zat, een reden is dat ze dit gedrag inzet. Op dit moment is een halsband of harnas aandoen en wandelen niet mogelijk. Dit dient in kleine stapjes te worden opgebouwd.
+Deze Siberische Husky van 2015 is actief, weet heel goed wat ze wil, en zeker ook wat ze niet wil. Ze kan niet bij andere dieren of bij kinderen. Ze heeft nood aan een fijne tuin om heerlijk in te spelen!
+</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Skippy</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/05/EVIOCLICK_14-10-25-1200x1800.jpg</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Skippy kwam bij ons terecht na een inbeslagname. Ze zat buiten tussen de rommel in een vieze ren.
+Skippy is een heuse furie. Als ze iets wil, gaat ze er voor de honderd procent voor. Aandacht? Spelen? Ze gooit zich volledig in de strijd. In die volle overgave wordt ze soms een beetje onhandig. Zo tuimelde ze bijvoorbeeld al eens van de bank. Maar ja, hoe zou je zelf zijn als je gepassioneerd bent door speeltjes?
+Het is niet omdat Skippy zo’n hevige dame is, dat ze niet kan genieten van een potje relaxen op zijn tijd. Een mand of zetel zijn héérlijke plekjes om dat te doen. Ze zal alleszins in de wolken zijn als ze binnenkort haar eigen relaxplekje heeft. Skippy kent trouwens al wat basiscommando’s zoals ZIT, AF en POOT.
+Ze is een mooie Duitse Herder van 4 jaar, maar ze mag wel wat kilootjes aankomen. Ze kan niet bij andere dieren of bij kleine kinderen en ze vereist een fijne tuin om in te relaxen. 
+Bied jij deze energieke herdershond een actief en liefdevol leven, dan wordt Skippy zeker en vast je beste vriendin!</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>11:26:42</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>11:29:44</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
file sync - fixed request recommendations - started styling suggestions page
</commit_message>
<xml_diff>
--- a/backend/records.xlsx
+++ b/backend/records.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:Q20"/>
@@ -726,6 +726,543 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4707522880</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Esco</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/06/IMG_7574-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>HALLO! Mijn naam is Esco en voordat ik verder vertel, laat ik me graag eerst even kriebelen door je. Je mag mij overal aaien, ik vind het heerlijk! Ik weet dat we elkaar nog niet kennen, maar dat maakt mij niet zoveel uit. Ik ben een echte allemansvriend!
+Ik zal iets meer vertellen over mezelf. Laat ik beginnen met te vertellen wat ik hier doe.
+Ik verdiende meer zorg dan dat ik kreeg, waardoor ik in beslag werd genomen. Nu zoek ik een nieuwe thuis en tot die tijd, gedraag ik me voorbeeldig in het asiel. In mijn kennel ben ik heel rustig en zeg ik iedereen netjes gedag wanneer ze aan mijn kennel staan.
+Mijn aandachtspunt is dat ik niet vriendelijk ben naar andere honden, maar ik compenseer dit ruimschoots door hartstikke vriendelijk te zijn naar mensen! Ik zou dus ook zeker bij grotere kinderen kunnen wonen. Als ze ook nog van voetbal of tennis houden, of me graag knuffelen, vind ik dat nóg fijner! Ik ben misschien niet meer de jongste, maar er is niets mis met mijn energieniveau.
+Ik zou graag willen wonen bij mensen zonder andere dieren. Omdat ik me zo goed gedraag, zou ik zelfs als eerste hond kunnen worden geplaatst! Een huis met een tuin is voor mij belangrijk, want als er veel mensen op straat wandelen met honden, blijf ik liever in de tuin.
+Wat heb ik te bieden? Miljoenen knuffels, likjes en gezelschap bij enge films.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Boelie</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/12/c66d6b76-c9b8-4598-b4e5-79e80c5440d5-1200x1600.jpg</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Deze knappe man is een kruising Akita met Amerikaanse Stafford. Hij is geboren in januari 2020. Zijn vorige eigenaar wilde hem na 6 dagen niet meer bij zich houden.
+Boelie is een actieve hond die graag dingen onderneemt. Toen hij hier binnenkwam, wist Boelie absoluut niet wat hij moest doen, hoe zich te gedragen en wat te verwachten. Er is in het asiel hard gewerkt aan zijn etiquette en tijdens het project Belgian Cell Dogs heeft Boelie laten zien een voorbeeldstudent te zijn. Zodra hij een band heeft met mensen (lees: wanneer er lekker eten te verdienen valt) heeft Boelie zin om te werken! Boelie heeft ook al geleerd om na te denken op momenten dat hij gefrustreerd wordt, daar waar hij voorheen kon happen. Hij heeft hier enorme vooruitgang in geboekt. We zijn dan ook heel enthousiast over zijn leervermogen!
+Favoriete bezigheden van deze vent zijn spelen en voerspelletjes. Momenten van aaien vindt hij ook fijn, maar Boelie is liever bezig met snuffelen, apporteren of snoepen. Oh, en als hobby is er ook nog zwemmen, of pootje baden. Zijn lijstje van favoriete bezigheden wordt afgesloten met een rustige wandeling.
+Boelie is een hele leergierige en voedselgerichte hond. Hij kent inmiddels de commando’s ‘zit’, ‘poot’ en ‘kom hier’.
+We zoeken voor Boelie een huis met een tuin. Zijn toekomstige baasje is het best in het begin meer thuis om hem te begeleiden. Oudere kinderen kunnen een optie voor hem zijn. Hij wordt helaas niet bij andere dieren geplaatst.
+Heeft u interesse in Boelie? Neem dan contact met ons op.
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Vicky</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/04/vickyyy-1-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Er zijn zo van die honden die bijna horen tot het ‘vaste meubilair’ van het asiel. Zonde, want we begrijpen vaak zelf niet goed hoe dat komt.
+Een van die honden is Mechelaar Vicky.
+Deze 7-jarige dame zit al bijna 3 jaar in ons asiel en ze zit samen met Molly in onze top drie van langzitters. Haar blinkende ogen verraden weinig over haar trieste verleden. Vicky’s leefruimte beperkte zich namelijk lang tot enkel een vieze ren.
+Vicky is ontzettend aanhankelijk, slim, energiek en speels. Ze houdt enorm van aandacht, maar heeft nog niet helemaal door dat je die best netjes vraagt. Aan de etiquette moet dus nog wat gewerkt worden. Je ziet Vicky heerlijk genieten van aaien, maar het allergelukkigste maak je haar door samen actief te zijn.
+Samen spelen in de tuin, speuren of trainen vindt ze heerlijk.
+Vicky is al goed getraind en doet het steeds beter aan de riem. Je begint wel best met wandelen in een rustige, prikkelarme omgeving. Het leven in huis kent ze nog niet, dus ze weet ook nog niet hoe ze met spullen in huis moet omgaan. Maar met het nodige geduld, leert slimme Vicky vast wel hoe ze zich als een echte dame moet gedragen.
+Vicky kan niet bij andere dieren of kleine kinderen. Ze heeft ook nood aan een grote omheinde tuin om lekker in rond te rennen. 
+Zoek je een energiek, aanhankelijk maatje dat je eerst vanop een veilig plekje kunt laten wennen aan het leven in huis? Dan is Vicky misschien wel de geknipte hond voor jou!
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>11:26:42</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>11:49:28</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4708839488</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Boelie</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/12/c66d6b76-c9b8-4598-b4e5-79e80c5440d5-1200x1600.jpg</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Deze knappe man is een kruising Akita met Amerikaanse Stafford. Hij is geboren in januari 2020. Zijn vorige eigenaar wilde hem na 6 dagen niet meer bij zich houden.
+Boelie is een actieve hond die graag dingen onderneemt. Toen hij hier binnenkwam, wist Boelie absoluut niet wat hij moest doen, hoe zich te gedragen en wat te verwachten. Er is in het asiel hard gewerkt aan zijn etiquette en tijdens het project Belgian Cell Dogs heeft Boelie laten zien een voorbeeldstudent te zijn. Zodra hij een band heeft met mensen (lees: wanneer er lekker eten te verdienen valt) heeft Boelie zin om te werken! Boelie heeft ook al geleerd om na te denken op momenten dat hij gefrustreerd wordt, daar waar hij voorheen kon happen. Hij heeft hier enorme vooruitgang in geboekt. We zijn dan ook heel enthousiast over zijn leervermogen!
+Favoriete bezigheden van deze vent zijn spelen en voerspelletjes. Momenten van aaien vindt hij ook fijn, maar Boelie is liever bezig met snuffelen, apporteren of snoepen. Oh, en als hobby is er ook nog zwemmen, of pootje baden. Zijn lijstje van favoriete bezigheden wordt afgesloten met een rustige wandeling.
+Boelie is een hele leergierige en voedselgerichte hond. Hij kent inmiddels de commando’s ‘zit’, ‘poot’ en ‘kom hier’.
+We zoeken voor Boelie een huis met een tuin. Zijn toekomstige baasje is het best in het begin meer thuis om hem te begeleiden. Oudere kinderen kunnen een optie voor hem zijn. Hij wordt helaas niet bij andere dieren geplaatst.
+Heeft u interesse in Boelie? Neem dan contact met ons op.
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Thor</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8797.1jpg-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Thor werd uit een donkere stal gehaald, helemaal achterin de tuin. Het was al even geleden dat Thor uit de stal was geweest: er werd niet gewandeld met Thor en ook in huis komen was geen optie. Sterker nog: op het moment dat Thor in beslag werd genomen, gaf de eigenaar al aan ‘Thor niet meer te willen’. Thor was in de ogen van zijn vorige eigenaar niet meer dan een object, waar hij in het asiel eindelijk weer ‘hond’ mocht zijn. Hij mocht zijn pootjes strekken, rondlopen in de speelweide en hij kreeg weer eens fysiek contact.
+Deze man is geboren in mei 2015 en zou graag de rest van zijn leven willen doorbrengen op een plaats waar hij wel graag gezien wordt, waar hij voldoende eten krijgt en waar hij goed verzorgd wordt.
+In het asiel heeft Thor onmiddellijk laten zien wat hij goed kan: hoog springen. Hij vond het zo fijn om zijn poten eens te kunnen strekken, dat hij dit iets té enthousiast heeft gedaan. Belangrijk punt voor zijn nieuwe eigenaren is dus een voldoende hoge omheining.
+Door al die jaren in duisternis te leven, waren heel veel dingen eng voor Thor. Hij heeft in het asiel veel geleerd: knuffels krijgen is heel leuk, wandelen is heel fijn en mensen dienen niet om je ergens in op te sluiten, maar om samen iets met je te doen!
+Waar Thor in het begin heel veel moeite had met alle prikkels in het asiel, zien we nu vreugde wanneer hij bekenden ziet. Hij begint te piepen en schudt met zijn hele achterwerk van enthousiasme!
+Een zindelijkheidstraining is voor Thor gewenst, evenals een huis met een tuin.
+Deze vriendelijke man moet nog veel leren, maar hij wil ontzettend graag! Bij rustige, geduldige mensen die in het begin meer thuis zijn, zal hij veel stappen kunnen zetten. Liefst ook letterlijk, want het leven opnieuw doorbrengen in een stal, is geen optie meer. Thor zou herplaatst kunnen worden bij een een stabiele en steriele teef.</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Esco</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/06/IMG_7574-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>HALLO! Mijn naam is Esco en voordat ik verder vertel, laat ik me graag eerst even kriebelen door je. Je mag mij overal aaien, ik vind het heerlijk! Ik weet dat we elkaar nog niet kennen, maar dat maakt mij niet zoveel uit. Ik ben een echte allemansvriend!
+Ik zal iets meer vertellen over mezelf. Laat ik beginnen met te vertellen wat ik hier doe.
+Ik verdiende meer zorg dan dat ik kreeg, waardoor ik in beslag werd genomen. Nu zoek ik een nieuwe thuis en tot die tijd, gedraag ik me voorbeeldig in het asiel. In mijn kennel ben ik heel rustig en zeg ik iedereen netjes gedag wanneer ze aan mijn kennel staan.
+Mijn aandachtspunt is dat ik niet vriendelijk ben naar andere honden, maar ik compenseer dit ruimschoots door hartstikke vriendelijk te zijn naar mensen! Ik zou dus ook zeker bij grotere kinderen kunnen wonen. Als ze ook nog van voetbal of tennis houden, of me graag knuffelen, vind ik dat nóg fijner! Ik ben misschien niet meer de jongste, maar er is niets mis met mijn energieniveau.
+Ik zou graag willen wonen bij mensen zonder andere dieren. Omdat ik me zo goed gedraag, zou ik zelfs als eerste hond kunnen worden geplaatst! Een huis met een tuin is voor mij belangrijk, want als er veel mensen op straat wandelen met honden, blijf ik liever in de tuin.
+Wat heb ik te bieden? Miljoenen knuffels, likjes en gezelschap bij enge films.</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>11:26:42</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>11:50:49</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4731860416</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Thor</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8797.1jpg-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Thor werd uit een donkere stal gehaald, helemaal achterin de tuin. Het was al even geleden dat Thor uit de stal was geweest: er werd niet gewandeld met Thor en ook in huis komen was geen optie. Sterker nog: op het moment dat Thor in beslag werd genomen, gaf de eigenaar al aan ‘Thor niet meer te willen’. Thor was in de ogen van zijn vorige eigenaar niet meer dan een object, waar hij in het asiel eindelijk weer ‘hond’ mocht zijn. Hij mocht zijn pootjes strekken, rondlopen in de speelweide en hij kreeg weer eens fysiek contact.
+Deze man is geboren in mei 2015 en zou graag de rest van zijn leven willen doorbrengen op een plaats waar hij wel graag gezien wordt, waar hij voldoende eten krijgt en waar hij goed verzorgd wordt.
+In het asiel heeft Thor onmiddellijk laten zien wat hij goed kan: hoog springen. Hij vond het zo fijn om zijn poten eens te kunnen strekken, dat hij dit iets té enthousiast heeft gedaan. Belangrijk punt voor zijn nieuwe eigenaren is dus een voldoende hoge omheining.
+Door al die jaren in duisternis te leven, waren heel veel dingen eng voor Thor. Hij heeft in het asiel veel geleerd: knuffels krijgen is heel leuk, wandelen is heel fijn en mensen dienen niet om je ergens in op te sluiten, maar om samen iets met je te doen!
+Waar Thor in het begin heel veel moeite had met alle prikkels in het asiel, zien we nu vreugde wanneer hij bekenden ziet. Hij begint te piepen en schudt met zijn hele achterwerk van enthousiasme!
+Een zindelijkheidstraining is voor Thor gewenst, evenals een huis met een tuin.
+Deze vriendelijke man moet nog veel leren, maar hij wil ontzettend graag! Bij rustige, geduldige mensen die in het begin meer thuis zijn, zal hij veel stappen kunnen zetten. Liefst ook letterlijk, want het leven opnieuw doorbrengen in een stal, is geen optie meer. Thor zou herplaatst kunnen worden bij een een stabiele en steriele teef.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Frankie</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/EVIOCLICK_14-10-11-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Frankie werd gevonden langs de gracht. Geen naam, geen exacte geboortedatum en geen chip.
+Hij was te mager en is onmiddellijk nagekeken door de dierenarts. Een oproep op Facebook heeft niets opgeleverd: zijn eigenaar heeft nooit naar hem gevraagd. Wellicht is dit voor hem beter, want hij kreeg absoluut niet de zorg die hij zou moeten krijgen.
+Deze knappe man heeft zich goed aangepast aan zijn nieuwe routine en reageerde vlot vriendelijk naar de verzorgers.
+Hij speelt dolgraag met tennisballen, waarbij hij ze met momenten terugbrengt en op andere momenten liever zelf speelt. Zijn atletisch vermogen komt op die momenten ook goed naar voren: hij springt zonder problemen op de zetel en op schoot.
+Commando’s zijn hem op dit moment nog onbekend, maar Frankie zou heel graag nieuwe dingen zien en leren! Hij is gek op lekker eten, dus trainen is zeker een mogelijkheid. Frankie’s favoriete bezigheid is, naast spelen en eten, knuffelen. Hij wordt door knuffelen heel rustig
+Een belangrijke regel bij Frankie is: wat van hem is, kan geruild worden. Afnemen vindt hij niet fijn.
+Voor deze knapperd zoeken we mensen die een huis met een tuin hebben. Een adoptie bij grotere kinderen en een stabiele teef is mogelijk.</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Dario</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/02/darioooo-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Dario werd gevonden in een losloopweide. Hij zou gewoond hebben op een plaats waar al meerdere honden in beslag werden genomen door een gebrek aan dierenwelzijn. Dat is niet verwonderlijk als we afgaan op zijn magere lijfje en onrustige karakter.
+Dario is een hond die met de nodige voorzichtigheid en wat geduld moet benaderd worden. Hij is vooral in het begin erg onzeker bij vreemde mensen, maar toch wint zijn nieuwsgierigheid het van zijn angst. Wanneer je zijn vertrouwen wint, laat hij je ook echt toe. Dan komt hij aandacht vragen en laat hij zich graag aaien.
+Er zit ook een echte speelvogel verscholen in Dario. Je doet hem een groot plezier met een balletje of pluchen beertje. Neem zijn speeltjes wel niet zomaar af, deze jongeman wil ruilen. Ook een partijtje touwtrekken ziet hij zeker zitten, al wordt hij dan soms iets te fanatiek. Opletten voor je vingers!
+Wanneer er snoepjes in beeld komen, is Dario helemaal in zijn nopjes. Hij haalt hiervoor al zijn charmes uit de kast en gaat flink zitten voor zijn beloning.
+Waar de culinaire wereld helemaal Dario zijn dada is, is de medische dat allesbehalve. Bij de dierenarts sloeg hij in een blinde paniek, wat zeker een aandachtspunt is voor zijn nieuwe eigenaren.
+Dario zijn nieuwe thuis is best een huis mét tuin, zodat deze pittige jongen zich buiten heerlijk kan uitleven. Hij kan niet geplaatst worden bij (kleine) kinderen. Grotere kinderen zijn zeker een optie. Ook een stabiele teef is eventueel een mogelijkheid.</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>11:26:42</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>11:54:58</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4731674880</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Thor</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8797.1jpg-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Thor werd uit een donkere stal gehaald, helemaal achterin de tuin. Het was al even geleden dat Thor uit de stal was geweest: er werd niet gewandeld met Thor en ook in huis komen was geen optie. Sterker nog: op het moment dat Thor in beslag werd genomen, gaf de eigenaar al aan ‘Thor niet meer te willen’. Thor was in de ogen van zijn vorige eigenaar niet meer dan een object, waar hij in het asiel eindelijk weer ‘hond’ mocht zijn. Hij mocht zijn pootjes strekken, rondlopen in de speelweide en hij kreeg weer eens fysiek contact.
+Deze man is geboren in mei 2015 en zou graag de rest van zijn leven willen doorbrengen op een plaats waar hij wel graag gezien wordt, waar hij voldoende eten krijgt en waar hij goed verzorgd wordt.
+In het asiel heeft Thor onmiddellijk laten zien wat hij goed kan: hoog springen. Hij vond het zo fijn om zijn poten eens te kunnen strekken, dat hij dit iets té enthousiast heeft gedaan. Belangrijk punt voor zijn nieuwe eigenaren is dus een voldoende hoge omheining.
+Door al die jaren in duisternis te leven, waren heel veel dingen eng voor Thor. Hij heeft in het asiel veel geleerd: knuffels krijgen is heel leuk, wandelen is heel fijn en mensen dienen niet om je ergens in op te sluiten, maar om samen iets met je te doen!
+Waar Thor in het begin heel veel moeite had met alle prikkels in het asiel, zien we nu vreugde wanneer hij bekenden ziet. Hij begint te piepen en schudt met zijn hele achterwerk van enthousiasme!
+Een zindelijkheidstraining is voor Thor gewenst, evenals een huis met een tuin.
+Deze vriendelijke man moet nog veel leren, maar hij wil ontzettend graag! Bij rustige, geduldige mensen die in het begin meer thuis zijn, zal hij veel stappen kunnen zetten. Liefst ook letterlijk, want het leven opnieuw doorbrengen in een stal, is geen optie meer. Thor zou herplaatst kunnen worden bij een een stabiele en steriele teef.</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Frankie</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/EVIOCLICK_14-10-11-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Frankie werd gevonden langs de gracht. Geen naam, geen exacte geboortedatum en geen chip.
+Hij was te mager en is onmiddellijk nagekeken door de dierenarts. Een oproep op Facebook heeft niets opgeleverd: zijn eigenaar heeft nooit naar hem gevraagd. Wellicht is dit voor hem beter, want hij kreeg absoluut niet de zorg die hij zou moeten krijgen.
+Deze knappe man heeft zich goed aangepast aan zijn nieuwe routine en reageerde vlot vriendelijk naar de verzorgers.
+Hij speelt dolgraag met tennisballen, waarbij hij ze met momenten terugbrengt en op andere momenten liever zelf speelt. Zijn atletisch vermogen komt op die momenten ook goed naar voren: hij springt zonder problemen op de zetel en op schoot.
+Commando’s zijn hem op dit moment nog onbekend, maar Frankie zou heel graag nieuwe dingen zien en leren! Hij is gek op lekker eten, dus trainen is zeker een mogelijkheid. Frankie’s favoriete bezigheid is, naast spelen en eten, knuffelen. Hij wordt door knuffelen heel rustig
+Een belangrijke regel bij Frankie is: wat van hem is, kan geruild worden. Afnemen vindt hij niet fijn.
+Voor deze knapperd zoeken we mensen die een huis met een tuin hebben. Een adoptie bij grotere kinderen en een stabiele teef is mogelijk.</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Dario</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/02/darioooo-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Dario werd gevonden in een losloopweide. Hij zou gewoond hebben op een plaats waar al meerdere honden in beslag werden genomen door een gebrek aan dierenwelzijn. Dat is niet verwonderlijk als we afgaan op zijn magere lijfje en onrustige karakter.
+Dario is een hond die met de nodige voorzichtigheid en wat geduld moet benaderd worden. Hij is vooral in het begin erg onzeker bij vreemde mensen, maar toch wint zijn nieuwsgierigheid het van zijn angst. Wanneer je zijn vertrouwen wint, laat hij je ook echt toe. Dan komt hij aandacht vragen en laat hij zich graag aaien.
+Er zit ook een echte speelvogel verscholen in Dario. Je doet hem een groot plezier met een balletje of pluchen beertje. Neem zijn speeltjes wel niet zomaar af, deze jongeman wil ruilen. Ook een partijtje touwtrekken ziet hij zeker zitten, al wordt hij dan soms iets te fanatiek. Opletten voor je vingers!
+Wanneer er snoepjes in beeld komen, is Dario helemaal in zijn nopjes. Hij haalt hiervoor al zijn charmes uit de kast en gaat flink zitten voor zijn beloning.
+Waar de culinaire wereld helemaal Dario zijn dada is, is de medische dat allesbehalve. Bij de dierenarts sloeg hij in een blinde paniek, wat zeker een aandachtspunt is voor zijn nieuwe eigenaren.
+Dario zijn nieuwe thuis is best een huis mét tuin, zodat deze pittige jongen zich buiten heerlijk kan uitleven. Hij kan niet geplaatst worden bij (kleine) kinderen. Grotere kinderen zijn zeker een optie. Ook een stabiele teef is eventueel een mogelijkheid.</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>11:26:42</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>11:55:41</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>4731676224</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Boelie</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/12/c66d6b76-c9b8-4598-b4e5-79e80c5440d5-1200x1600.jpg</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Deze knappe man is een kruising Akita met Amerikaanse Stafford. Hij is geboren in januari 2020. Zijn vorige eigenaar wilde hem na 6 dagen niet meer bij zich houden.
+Boelie is een actieve hond die graag dingen onderneemt. Toen hij hier binnenkwam, wist Boelie absoluut niet wat hij moest doen, hoe zich te gedragen en wat te verwachten. Er is in het asiel hard gewerkt aan zijn etiquette en tijdens het project Belgian Cell Dogs heeft Boelie laten zien een voorbeeldstudent te zijn. Zodra hij een band heeft met mensen (lees: wanneer er lekker eten te verdienen valt) heeft Boelie zin om te werken! Boelie heeft ook al geleerd om na te denken op momenten dat hij gefrustreerd wordt, daar waar hij voorheen kon happen. Hij heeft hier enorme vooruitgang in geboekt. We zijn dan ook heel enthousiast over zijn leervermogen!
+Favoriete bezigheden van deze vent zijn spelen en voerspelletjes. Momenten van aaien vindt hij ook fijn, maar Boelie is liever bezig met snuffelen, apporteren of snoepen. Oh, en als hobby is er ook nog zwemmen, of pootje baden. Zijn lijstje van favoriete bezigheden wordt afgesloten met een rustige wandeling.
+Boelie is een hele leergierige en voedselgerichte hond. Hij kent inmiddels de commando’s ‘zit’, ‘poot’ en ‘kom hier’.
+We zoeken voor Boelie een huis met een tuin. Zijn toekomstige baasje is het best in het begin meer thuis om hem te begeleiden. Oudere kinderen kunnen een optie voor hem zijn. Hij wordt helaas niet bij andere dieren geplaatst.
+Heeft u interesse in Boelie? Neem dan contact met ons op.
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Thor</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8797.1jpg-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Thor werd uit een donkere stal gehaald, helemaal achterin de tuin. Het was al even geleden dat Thor uit de stal was geweest: er werd niet gewandeld met Thor en ook in huis komen was geen optie. Sterker nog: op het moment dat Thor in beslag werd genomen, gaf de eigenaar al aan ‘Thor niet meer te willen’. Thor was in de ogen van zijn vorige eigenaar niet meer dan een object, waar hij in het asiel eindelijk weer ‘hond’ mocht zijn. Hij mocht zijn pootjes strekken, rondlopen in de speelweide en hij kreeg weer eens fysiek contact.
+Deze man is geboren in mei 2015 en zou graag de rest van zijn leven willen doorbrengen op een plaats waar hij wel graag gezien wordt, waar hij voldoende eten krijgt en waar hij goed verzorgd wordt.
+In het asiel heeft Thor onmiddellijk laten zien wat hij goed kan: hoog springen. Hij vond het zo fijn om zijn poten eens te kunnen strekken, dat hij dit iets té enthousiast heeft gedaan. Belangrijk punt voor zijn nieuwe eigenaren is dus een voldoende hoge omheining.
+Door al die jaren in duisternis te leven, waren heel veel dingen eng voor Thor. Hij heeft in het asiel veel geleerd: knuffels krijgen is heel leuk, wandelen is heel fijn en mensen dienen niet om je ergens in op te sluiten, maar om samen iets met je te doen!
+Waar Thor in het begin heel veel moeite had met alle prikkels in het asiel, zien we nu vreugde wanneer hij bekenden ziet. Hij begint te piepen en schudt met zijn hele achterwerk van enthousiasme!
+Een zindelijkheidstraining is voor Thor gewenst, evenals een huis met een tuin.
+Deze vriendelijke man moet nog veel leren, maar hij wil ontzettend graag! Bij rustige, geduldige mensen die in het begin meer thuis zijn, zal hij veel stappen kunnen zetten. Liefst ook letterlijk, want het leven opnieuw doorbrengen in een stal, is geen optie meer. Thor zou herplaatst kunnen worden bij een een stabiele en steriele teef.</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Frankie</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/EVIOCLICK_14-10-11-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Frankie werd gevonden langs de gracht. Geen naam, geen exacte geboortedatum en geen chip.
+Hij was te mager en is onmiddellijk nagekeken door de dierenarts. Een oproep op Facebook heeft niets opgeleverd: zijn eigenaar heeft nooit naar hem gevraagd. Wellicht is dit voor hem beter, want hij kreeg absoluut niet de zorg die hij zou moeten krijgen.
+Deze knappe man heeft zich goed aangepast aan zijn nieuwe routine en reageerde vlot vriendelijk naar de verzorgers.
+Hij speelt dolgraag met tennisballen, waarbij hij ze met momenten terugbrengt en op andere momenten liever zelf speelt. Zijn atletisch vermogen komt op die momenten ook goed naar voren: hij springt zonder problemen op de zetel en op schoot.
+Commando’s zijn hem op dit moment nog onbekend, maar Frankie zou heel graag nieuwe dingen zien en leren! Hij is gek op lekker eten, dus trainen is zeker een mogelijkheid. Frankie’s favoriete bezigheid is, naast spelen en eten, knuffelen. Hij wordt door knuffelen heel rustig
+Een belangrijke regel bij Frankie is: wat van hem is, kan geruild worden. Afnemen vindt hij niet fijn.
+Voor deze knapperd zoeken we mensen die een huis met een tuin hebben. Een adoptie bij grotere kinderen en een stabiele teef is mogelijk.</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>11:26:42</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>11:56:42</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug fixes, version that works!
</commit_message>
<xml_diff>
--- a/backend/records.xlsx
+++ b/backend/records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nam/PycharmProjects/HCIPaper/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9985B7C-62BD-CC4F-A4E4-2AD3BE784BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34149634-2BC8-9E44-AEF6-D905D046E5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="4160" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7860" yWindow="2660" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:T14"/>
+      <selection activeCell="A2" sqref="A2:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>